<commit_message>
Replace placeholder data in IHDbT
</commit_message>
<xml_diff>
--- a/InputData/indst/IHDbT/Indst Heat Demand by Temp.xlsx
+++ b/InputData/indst/IHDbT/Indst Heat Demand by Temp.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\indst\IHDbT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\indst\IHDbT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645DDD2F-2085-4394-B35D-1787314EAF20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C93C8E-FEF1-4AF0-944B-3A32143010E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15780" yWindow="990" windowWidth="26865" windowHeight="20775" xr2:uid="{9AA6BDF2-7B91-4567-88A2-0D83F9E3E450}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9AA6BDF2-7B91-4567-88A2-0D83F9E3E450}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,21 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
-  <calcPr calcId="191029"/>
+  <definedNames>
+    <definedName name="CH4_to_CO2e">'[1]Cross-Page Data'!$C$12</definedName>
+    <definedName name="cpi_2010to2012">#REF!</definedName>
+    <definedName name="cpi_2013to2012">#REF!</definedName>
+    <definedName name="cpi_2014to2012">#REF!</definedName>
+    <definedName name="cpi_2016to2012">#REF!</definedName>
+    <definedName name="gigwatts_to_megawatts">[3]About!$A$31</definedName>
+    <definedName name="N2O_to_CO2e">'[1]Cross-Page Data'!$C$13</definedName>
+    <definedName name="unit_conv">[4]About!$A$123</definedName>
+  </definedNames>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,14 +53,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
   <si>
     <t>IHDbT Industrial Heat Demand by Temperature</t>
   </si>
   <si>
-    <t>Fraunhofer Institute</t>
-  </si>
-  <si>
     <t>Mapping and analyses of the current and future (2020 - 2030) heating/cooling fuel deployment (fossil/renewables)</t>
   </si>
   <si>
@@ -141,9 +151,6 @@
     <t>All Industries (Total)</t>
   </si>
   <si>
-    <t>Source:</t>
-  </si>
-  <si>
     <t>Unit: dimensionless</t>
   </si>
   <si>
@@ -226,6 +233,21 @@
   </si>
   <si>
     <t>Perc Medium and High Temp</t>
+  </si>
+  <si>
+    <t>We assume the fraction of low temp heat is 100% for the agriculture, natural gas processing, water and waste,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">and construction industries. </t>
+  </si>
+  <si>
+    <t>Sources:</t>
+  </si>
+  <si>
+    <t>Fraunhofer Institute (all industries except refining)</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -276,7 +298,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,7 +313,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -310,13 +338,9 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -330,7 +354,20 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -3415,180 +3452,292 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Main Source"/>
-      <sheetName val="Alternate Source"/>
+      <sheetName val="About"/>
+      <sheetName val="Cross-Page Data"/>
+      <sheetName val="Non-Energy FF CO2 Emissions"/>
+      <sheetName val="Cement CO2 Emissions"/>
+      <sheetName val="Iron and Steel"/>
+      <sheetName val="Coal Mining"/>
+      <sheetName val="Natural Gas Systems"/>
+      <sheetName val="Petroleum Systems"/>
+      <sheetName val="Chem - HCFC 22 Production"/>
+      <sheetName val="Chem - ODS"/>
+      <sheetName val="Other - Aluminum"/>
+      <sheetName val="Other - Magnesium"/>
+      <sheetName val="Other - Semiconductor Mfg"/>
+      <sheetName val="Other - Elec Trans and Dist"/>
+      <sheetName val="Agriculture - EF &amp; Manure Mgmt"/>
+      <sheetName val="Agriculture - Rice Cultivation"/>
+      <sheetName val="Agriculture - Soil Mgmt"/>
+      <sheetName val="Waste - Landfills"/>
+      <sheetName val="Waste - Water Treatment"/>
+      <sheetName val="Other Industrial Processes"/>
+      <sheetName val="Combined Data"/>
+      <sheetName val="BPEiC-CO2"/>
+      <sheetName val="BPEiC-CH4"/>
+      <sheetName val="BPEiC-N2O"/>
+      <sheetName val="BPEiC-F-gases"/>
+      <sheetName val="EPA (2017) Table A3.6-1"/>
+      <sheetName val="EPA (2017) Table A3.6-7"/>
+      <sheetName val="EPA (2017) Table A3.6-10"/>
+      <sheetName val="AEO 2017_Table 6"/>
+      <sheetName val="AEO 2017_Table 11"/>
+      <sheetName val="AEO 2017_Table 13"/>
+      <sheetName val="AEO 2017_Table 15"/>
+      <sheetName val="AEO 2017_Table 19"/>
+      <sheetName val="AEO 2017_Table 20"/>
+      <sheetName val="AEO 2017_Table 24"/>
+      <sheetName val="AEO 2017_Table 62"/>
+      <sheetName val="AEO 2016_Table 6"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="12">
+          <cell r="C12">
+            <v>28</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="C13">
+            <v>265</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9">
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>Transport Refrigeration</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Table of Contents"/>
+      <sheetName val="Indst Fuel Switching"/>
+      <sheetName val="Hydrogen Production"/>
+      <sheetName val="F-gases"/>
+      <sheetName val="Non-f-gas Process Emissions"/>
+      <sheetName val="Indst Efficiency"/>
+      <sheetName val="Industry CCS"/>
+      <sheetName val="Material Efficiency"/>
+      <sheetName val="CES"/>
+      <sheetName val="Battery Storage"/>
+      <sheetName val="Transmission"/>
+      <sheetName val="Demand Response"/>
+      <sheetName val="Coal regs"/>
+      <sheetName val="Gas regs"/>
+      <sheetName val="Nuclear subsidy"/>
+      <sheetName val="ITC and PTC"/>
+      <sheetName val="ZEV std"/>
+      <sheetName val="EV Tax Credits"/>
+      <sheetName val="Trans fuel econ"/>
+      <sheetName val="Mode shifting"/>
+      <sheetName val="EV charging"/>
+      <sheetName val="Bldg Electrification"/>
+      <sheetName val="Bldg Rebates"/>
+      <sheetName val="Bldg Retrofits"/>
+      <sheetName val="Bldg Efficiency"/>
+      <sheetName val="Forest Policies"/>
+      <sheetName val="Supporting Data --&gt;"/>
+      <sheetName val="NREL Indst"/>
+      <sheetName val="AEO 2021 Table 5"/>
+      <sheetName val="AEO 2021 Table 6"/>
+      <sheetName val="AEO 2021 Table 7"/>
+      <sheetName val="AEO 2021 Table 21"/>
+      <sheetName val="AEO 2021 Table 22"/>
+      <sheetName val="AEO 2021 Table 39"/>
+      <sheetName val="AEO 2018 Table 47"/>
+      <sheetName val="AEO 2017 Table 7"/>
+      <sheetName val="AEO 2017 Table 50"/>
+      <sheetName val="AEO2015 Table 7"/>
+      <sheetName val="AEO20212 Table 7"/>
+      <sheetName val="EIA Appl Data"/>
+      <sheetName val="USCA HFCs"/>
+      <sheetName val="Conversion Factors"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38"/>
+      <sheetData sheetId="39"/>
+      <sheetData sheetId="40"/>
+      <sheetData sheetId="41"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="About"/>
+      <sheetName val="2035 Report Deployment"/>
+      <sheetName val="2035 Report Data"/>
+      <sheetName val="EPS Output"/>
+      <sheetName val="AEO Table 9"/>
+      <sheetName val="AEO Table 9 (2019)"/>
+      <sheetName val="AEO Table 16"/>
+      <sheetName val="BGBSC"/>
+      <sheetName val="PAGBSC"/>
+      <sheetName val="SYGBSC"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="70">
-          <cell r="B70" t="str">
-            <v>&gt;500 °C</v>
-          </cell>
-          <cell r="C70" t="str">
-            <v>200-500 °C</v>
-          </cell>
-          <cell r="D70" t="str">
-            <v>100-200 °C</v>
-          </cell>
-          <cell r="E70" t="str">
-            <v>&lt;100 °C</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="A71" t="str">
-            <v>All Industries (Total)</v>
-          </cell>
-          <cell r="B71">
-            <v>3641.1399442309016</v>
-          </cell>
-          <cell r="C71">
-            <v>632.1033904211838</v>
-          </cell>
-          <cell r="D71">
-            <v>1808.414137684274</v>
-          </cell>
-          <cell r="E71">
-            <v>826.59674132000964</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="A72" t="str">
-            <v>Iron &amp; Steel</v>
-          </cell>
-          <cell r="B72">
-            <v>1752.3102864634591</v>
-          </cell>
-          <cell r="C72">
-            <v>56.103851220815123</v>
-          </cell>
-          <cell r="D72">
-            <v>0</v>
-          </cell>
-          <cell r="E72">
-            <v>56.103851220815123</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="A73" t="str">
-            <v>Nonmetallic Minerals</v>
-          </cell>
-          <cell r="B73">
-            <v>854.64866693041711</v>
-          </cell>
-          <cell r="C73">
-            <v>168.31155366244539</v>
-          </cell>
-          <cell r="D73">
-            <v>112.20770244163025</v>
-          </cell>
-          <cell r="E73">
-            <v>28.051925610407562</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="A74" t="str">
-            <v>Chemicals</v>
-          </cell>
-          <cell r="B74">
-            <v>895.79149115901475</v>
-          </cell>
-          <cell r="C74">
-            <v>28.051925610407562</v>
-          </cell>
-          <cell r="D74">
-            <v>140.25962805203781</v>
-          </cell>
-          <cell r="E74">
-            <v>280.51925610407562</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="A75" t="str">
-            <v>Nonferrous Metals</v>
-          </cell>
-          <cell r="B75">
-            <v>84.155776831222695</v>
-          </cell>
-          <cell r="C75">
-            <v>56.103851220815123</v>
-          </cell>
-          <cell r="D75">
-            <v>14.961026992217368</v>
-          </cell>
-          <cell r="E75">
-            <v>28.051925610407562</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="A76" t="str">
-            <v>Food &amp; Beverage</v>
-          </cell>
-          <cell r="B76">
-            <v>41.14282422859776</v>
-          </cell>
-          <cell r="C76">
-            <v>56.103851220815123</v>
-          </cell>
-          <cell r="D76">
-            <v>209.45437789104312</v>
-          </cell>
-          <cell r="E76">
-            <v>211.32450626507031</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="A77" t="str">
-            <v>Pulp &amp; Paper</v>
-          </cell>
-          <cell r="B77">
-            <v>13.090898618190195</v>
-          </cell>
-          <cell r="C77">
-            <v>43.012952602624928</v>
-          </cell>
-          <cell r="D77">
-            <v>714.38903887837921</v>
-          </cell>
-          <cell r="E77">
-            <v>97.246675449412891</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="A78" t="str">
-            <v>Machinery &amp; Vehicles</v>
-          </cell>
-          <cell r="B78">
-            <v>0</v>
-          </cell>
-          <cell r="C78">
-            <v>28.051925610407562</v>
-          </cell>
-          <cell r="D78">
-            <v>99.116803823440051</v>
-          </cell>
-          <cell r="E78">
-            <v>41.14282422859776</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="A79" t="str">
-            <v>Other Industries</v>
-          </cell>
-          <cell r="B79">
-            <v>0</v>
-          </cell>
-          <cell r="C79">
-            <v>196.36347927285294</v>
-          </cell>
-          <cell r="D79">
-            <v>518.02555960552627</v>
-          </cell>
-          <cell r="E79">
-            <v>84.155776831222695</v>
+        <row r="31">
+          <cell r="A31">
+            <v>1000</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="About"/>
+      <sheetName val="Country Selector"/>
+      <sheetName val="Multipliers and Adjustments"/>
+      <sheetName val="EPA Data"/>
+      <sheetName val="Tech to Policy Mapping"/>
+      <sheetName val="SNAP Adjustment"/>
+      <sheetName val="Cement Data"/>
+      <sheetName val="Data Check"/>
+      <sheetName val="PERAC-cement"/>
+      <sheetName val="PERAC-ngps-mthncptr"/>
+      <sheetName val="PERAC-ngps-mthndstr"/>
+      <sheetName val="PERAC-fgassubstitution"/>
+      <sheetName val="PERAC-fgasdestruction"/>
+      <sheetName val="PERAC-fgasrecovery"/>
+      <sheetName val="PERAC-inspctmaintretrofit"/>
+      <sheetName val="PERAC-coalmining-mthncptr"/>
+      <sheetName val="PERAC-coalmining-mthndstr"/>
+      <sheetName val="PERAC-waste-mthncptr"/>
+      <sheetName val="PERAC-waste-mthndstr"/>
+      <sheetName val="PERAC-cropsrice"/>
+      <sheetName val="PERAC-livestock"/>
+      <sheetName val="PERAC-MCD"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="123">
+          <cell r="A123">
+            <v>1000000000000</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3891,43 +4040,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE5FEEC-01CE-4291-999E-35B30A1256CF}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="85.08984375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" s="14">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B5" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="B6" s="15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B7" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>4</v>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -3943,472 +4112,472 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADCAD35F-524E-466F-828E-86F7D1F08980}">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="5" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="2" max="5" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B38" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="1" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="B39" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="C39" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="D39" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="E39" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E39" s="7" t="s">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="B40" s="6">
+        <v>93.7</v>
+      </c>
+      <c r="C40" s="6">
+        <v>3</v>
+      </c>
+      <c r="D40" s="6">
+        <v>0</v>
+      </c>
+      <c r="E40" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="8">
-        <v>93.7</v>
-      </c>
-      <c r="C40" s="8">
+      <c r="B41" s="6">
+        <v>45.7</v>
+      </c>
+      <c r="C41" s="6">
+        <v>9</v>
+      </c>
+      <c r="D41" s="6">
+        <v>6</v>
+      </c>
+      <c r="E41" s="6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="6">
+        <v>47.9</v>
+      </c>
+      <c r="C42" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="D42" s="6">
+        <v>7.5</v>
+      </c>
+      <c r="E42" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="C43" s="6">
         <v>3</v>
       </c>
-      <c r="D40" s="8">
+      <c r="D43" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="E43" s="6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C44" s="6">
+        <v>3</v>
+      </c>
+      <c r="D44" s="6">
+        <v>11.2</v>
+      </c>
+      <c r="E44" s="6">
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="C45" s="6">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D45" s="6">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="E45" s="6">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" s="6">
         <v>0</v>
       </c>
-      <c r="E40" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>17</v>
-      </c>
-      <c r="B41" s="8">
-        <v>45.7</v>
-      </c>
-      <c r="C41" s="8">
-        <v>9</v>
-      </c>
-      <c r="D41" s="8">
-        <v>6</v>
-      </c>
-      <c r="E41" s="8">
+      <c r="C46" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>18</v>
-      </c>
-      <c r="B42" s="8">
-        <v>47.9</v>
-      </c>
-      <c r="C42" s="8">
-        <v>1.5</v>
-      </c>
-      <c r="D42" s="8">
-        <v>7.5</v>
-      </c>
-      <c r="E42" s="8">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>19</v>
-      </c>
-      <c r="B43" s="8">
+      <c r="D46" s="6">
+        <v>5.3</v>
+      </c>
+      <c r="E46" s="6">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" s="6">
+        <v>0</v>
+      </c>
+      <c r="C47" s="6">
+        <v>10.5</v>
+      </c>
+      <c r="D47" s="6">
+        <v>27.7</v>
+      </c>
+      <c r="E47" s="6">
         <v>4.5</v>
       </c>
-      <c r="C43" s="8">
-        <v>3</v>
-      </c>
-      <c r="D43" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="E43" s="8">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>20</v>
-      </c>
-      <c r="B44" s="8">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C44" s="8">
-        <v>3</v>
-      </c>
-      <c r="D44" s="8">
-        <v>11.2</v>
-      </c>
-      <c r="E44" s="8">
-        <v>11.3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>21</v>
-      </c>
-      <c r="B45" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="C45" s="8">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D45" s="8">
-        <v>38.200000000000003</v>
-      </c>
-      <c r="E45" s="8">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>22</v>
-      </c>
-      <c r="B46" s="8">
-        <v>0</v>
-      </c>
-      <c r="C46" s="8">
-        <v>1.5</v>
-      </c>
-      <c r="D46" s="8">
-        <v>5.3</v>
-      </c>
-      <c r="E46" s="8">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B47" s="8">
-        <v>0</v>
-      </c>
-      <c r="C47" s="8">
-        <v>10.5</v>
-      </c>
-      <c r="D47" s="8">
-        <v>27.7</v>
-      </c>
-      <c r="E47" s="8">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>25</v>
       </c>
       <c r="B51">
         <v>115.5</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B52">
         <v>600</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B54">
         <f>B52/B51</f>
         <v>5.1948051948051948</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B55">
         <f>E55/E56</f>
         <v>3.5999971200023038</v>
       </c>
       <c r="D55" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E55">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D56" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E56">
         <v>0.27777800000000002</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B60" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B62" s="9">
+      <c r="B62" s="7">
         <f>SUM(B63:B70)</f>
         <v>3641.1399442309016</v>
       </c>
-      <c r="C62" s="9">
+      <c r="C62" s="7">
         <f>SUM(C63:C70)</f>
         <v>632.1033904211838</v>
       </c>
-      <c r="D62" s="9">
+      <c r="D62" s="7">
         <f>SUM(D63:D70)</f>
         <v>1808.414137684274</v>
       </c>
-      <c r="E62" s="9">
+      <c r="E62" s="7">
         <f>SUM(E63:E70)</f>
         <v>826.59674132000964</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="str">
         <f t="shared" ref="A63:A70" si="0">A40</f>
         <v>Iron &amp; Steel</v>
       </c>
-      <c r="B63" s="10">
+      <c r="B63" s="8">
         <f t="shared" ref="B63:E70" si="1">B40*$B$54*$B$55</f>
         <v>1752.3102864634591</v>
       </c>
-      <c r="C63" s="10">
+      <c r="C63" s="8">
         <f t="shared" si="1"/>
         <v>56.103851220815123</v>
       </c>
-      <c r="D63" s="10">
+      <c r="D63" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E63" s="10">
+      <c r="E63" s="8">
         <f t="shared" si="1"/>
         <v>56.103851220815123</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="str">
         <f t="shared" si="0"/>
         <v>Nonmetallic Minerals</v>
       </c>
-      <c r="B64" s="10">
+      <c r="B64" s="8">
         <f t="shared" si="1"/>
         <v>854.64866693041711</v>
       </c>
-      <c r="C64" s="10">
+      <c r="C64" s="8">
         <f t="shared" si="1"/>
         <v>168.31155366244539</v>
       </c>
-      <c r="D64" s="10">
+      <c r="D64" s="8">
         <f t="shared" si="1"/>
         <v>112.20770244163025</v>
       </c>
-      <c r="E64" s="10">
+      <c r="E64" s="8">
         <f t="shared" si="1"/>
         <v>28.051925610407562</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="str">
         <f t="shared" si="0"/>
         <v>Chemicals</v>
       </c>
-      <c r="B65" s="10">
+      <c r="B65" s="8">
         <f t="shared" si="1"/>
         <v>895.79149115901475</v>
       </c>
-      <c r="C65" s="10">
+      <c r="C65" s="8">
         <f t="shared" si="1"/>
         <v>28.051925610407562</v>
       </c>
-      <c r="D65" s="10">
+      <c r="D65" s="8">
         <f t="shared" si="1"/>
         <v>140.25962805203781</v>
       </c>
-      <c r="E65" s="10">
+      <c r="E65" s="8">
         <f t="shared" si="1"/>
         <v>280.51925610407562</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="str">
         <f t="shared" si="0"/>
         <v>Nonferrous Metals</v>
       </c>
-      <c r="B66" s="10">
+      <c r="B66" s="8">
         <f t="shared" si="1"/>
         <v>84.155776831222695</v>
       </c>
-      <c r="C66" s="10">
+      <c r="C66" s="8">
         <f t="shared" si="1"/>
         <v>56.103851220815123</v>
       </c>
-      <c r="D66" s="10">
+      <c r="D66" s="8">
         <f t="shared" si="1"/>
         <v>14.961026992217368</v>
       </c>
-      <c r="E66" s="10">
+      <c r="E66" s="8">
         <f t="shared" si="1"/>
         <v>28.051925610407562</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="str">
         <f t="shared" si="0"/>
         <v>Food &amp; Beverage</v>
       </c>
-      <c r="B67" s="10">
+      <c r="B67" s="8">
         <f t="shared" si="1"/>
         <v>41.14282422859776</v>
       </c>
-      <c r="C67" s="10">
+      <c r="C67" s="8">
         <f t="shared" si="1"/>
         <v>56.103851220815123</v>
       </c>
-      <c r="D67" s="10">
+      <c r="D67" s="8">
         <f t="shared" si="1"/>
         <v>209.45437789104312</v>
       </c>
-      <c r="E67" s="10">
+      <c r="E67" s="8">
         <f t="shared" si="1"/>
         <v>211.32450626507031</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" t="str">
         <f t="shared" si="0"/>
         <v>Pulp &amp; Paper</v>
       </c>
-      <c r="B68" s="10">
+      <c r="B68" s="8">
         <f t="shared" si="1"/>
         <v>13.090898618190195</v>
       </c>
-      <c r="C68" s="10">
+      <c r="C68" s="8">
         <f t="shared" si="1"/>
         <v>43.012952602624928</v>
       </c>
-      <c r="D68" s="10">
+      <c r="D68" s="8">
         <f t="shared" si="1"/>
         <v>714.38903887837921</v>
       </c>
-      <c r="E68" s="10">
+      <c r="E68" s="8">
         <f t="shared" si="1"/>
         <v>97.246675449412891</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="str">
         <f t="shared" si="0"/>
         <v>Machinery &amp; Vehicles</v>
       </c>
-      <c r="B69" s="10">
+      <c r="B69" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C69" s="10">
+      <c r="C69" s="8">
         <f t="shared" si="1"/>
         <v>28.051925610407562</v>
       </c>
-      <c r="D69" s="10">
+      <c r="D69" s="8">
         <f t="shared" si="1"/>
         <v>99.116803823440051</v>
       </c>
-      <c r="E69" s="10">
+      <c r="E69" s="8">
         <f t="shared" si="1"/>
         <v>41.14282422859776</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="str">
         <f t="shared" si="0"/>
         <v>Other Industries</v>
       </c>
-      <c r="B70" s="10">
+      <c r="B70" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C70" s="10">
+      <c r="C70" s="8">
         <f t="shared" si="1"/>
         <v>196.36347927285294</v>
       </c>
-      <c r="D70" s="10">
+      <c r="D70" s="8">
         <f t="shared" si="1"/>
         <v>518.02555960552627</v>
       </c>
-      <c r="E70" s="10">
+      <c r="E70" s="8">
         <f t="shared" si="1"/>
         <v>84.155776831222695</v>
       </c>
@@ -4426,324 +4595,346 @@
   </sheetPr>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:B13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="46.28515625" customWidth="1"/>
+    <col min="1" max="1" width="46.26953125" customWidth="1"/>
     <col min="2" max="3" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="12">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10">
+        <f t="shared" ref="C2:C14" si="0">1-B2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B3" s="11">
+        <f>$B$23</f>
+        <v>0.75409836065573765</v>
+      </c>
+      <c r="C3" s="10">
+        <f t="shared" si="0"/>
+        <v>0.24590163934426235</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="C2" s="12">
-        <f t="shared" ref="C2:C14" si="0">1-B2</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B4" s="11">
+        <f t="shared" ref="B4:B5" si="1">$B$23</f>
+        <v>0.75409836065573765</v>
+      </c>
+      <c r="C4" s="10">
+        <f t="shared" si="0"/>
+        <v>0.24590163934426235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="C3" s="12">
+      <c r="B5" s="11">
+        <f t="shared" si="1"/>
+        <v>0.75409836065573765</v>
+      </c>
+      <c r="C5" s="10">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+        <v>0.24590163934426235</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="C4" s="12">
+      <c r="B6" s="11">
+        <f>SUM(Data!D67:E67)/SUM(Data!B67:E67)</f>
+        <v>0.81227436823104693</v>
+      </c>
+      <c r="C6" s="10">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+        <v>0.18772563176895307</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="C5" s="12">
+      <c r="B7" s="11">
+        <f>$B$23</f>
+        <v>0.75409836065573765</v>
+      </c>
+      <c r="C7" s="10">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+        <v>0.24590163934426235</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="C6" s="12">
+      <c r="B8" s="11">
+        <f>$B$23</f>
+        <v>0.75409836065573765</v>
+      </c>
+      <c r="C8" s="10">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+        <v>0.24590163934426235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="C7" s="12">
+      <c r="B9" s="11">
+        <f>SUM(Data!D68:E68)/SUM(Data!B68:E68)</f>
+        <v>0.93534482758620685</v>
+      </c>
+      <c r="C9" s="10">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+        <v>6.4655172413793149E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="C8" s="12">
+      <c r="B10" s="11">
+        <f>$B$23</f>
+        <v>0.75409836065573765</v>
+      </c>
+      <c r="C10" s="10">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+        <v>0.24590163934426235</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="C9" s="12">
+      <c r="B11" s="11">
+        <f>SUM(Data!D65:E65)/SUM(Data!B65:E65)</f>
+        <v>0.31293463143254524</v>
+      </c>
+      <c r="C11" s="10">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+        <v>0.68706536856745482</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="C10" s="12">
+      <c r="B12" s="11">
+        <f>$B$23</f>
+        <v>0.75409836065573765</v>
+      </c>
+      <c r="C12" s="10">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+        <v>0.24590163934426235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="C11" s="12">
+      <c r="B13" s="11">
+        <f>$B$23</f>
+        <v>0.75409836065573765</v>
+      </c>
+      <c r="C13" s="10">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+        <v>0.24590163934426235</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="C12" s="12">
+      <c r="B14" s="10">
+        <f>SUM(Data!D64:E64)/SUM(Data!B64:E64)</f>
+        <v>0.12057877813504822</v>
+      </c>
+      <c r="C14" s="10">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+        <v>0.87942122186495175</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="C13" s="12">
-        <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="C14" s="12">
-        <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="12">
+      <c r="B15" s="10">
         <f>SUM(Data!D63:E63)/SUM(Data!B63:E63)</f>
         <v>3.0090270812437311E-2</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="10">
         <f>1-B15</f>
         <v>0.96990972918756269</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="11">
+        <f>SUM(Data!D66:E66)/SUM(Data!B66:E66)</f>
+        <v>0.23469387755102042</v>
+      </c>
+      <c r="C16" s="10">
+        <f t="shared" ref="C16:C26" si="2">1-B16</f>
+        <v>0.76530612244897955</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="11">
+        <f>$B$23</f>
+        <v>0.75409836065573765</v>
+      </c>
+      <c r="C17" s="10">
+        <f t="shared" si="2"/>
+        <v>0.24590163934426235</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="C16" s="12">
-        <f t="shared" ref="C16:C26" si="1">1-B16</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B18" s="11">
+        <f t="shared" ref="B18:B19" si="3">$B$23</f>
+        <v>0.75409836065573765</v>
+      </c>
+      <c r="C18" s="10">
+        <f t="shared" si="2"/>
+        <v>0.24590163934426235</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="C17" s="12">
-        <f t="shared" si="1"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B19" s="11">
+        <f t="shared" si="3"/>
+        <v>0.75409836065573765</v>
+      </c>
+      <c r="C19" s="10">
+        <f t="shared" si="2"/>
+        <v>0.24590163934426235</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="C18" s="12">
-        <f t="shared" si="1"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B20" s="11">
+        <f>SUM(Data!D69:E69)/SUM(Data!B69:E69)</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C20" s="10">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666663</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="C19" s="12">
-        <f t="shared" si="1"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B21" s="11">
+        <f>$B$20</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C21" s="10">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666663</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="C20" s="12">
-        <f t="shared" si="1"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B22" s="11">
+        <f>$B$20</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C22" s="10">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666663</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="C21" s="12">
-        <f t="shared" si="1"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B23" s="11">
+        <f>SUM(Data!D70:E70)/SUM(Data!B70:E70)</f>
+        <v>0.75409836065573765</v>
+      </c>
+      <c r="C23" s="10">
+        <f t="shared" si="2"/>
+        <v>0.24590163934426235</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="C22" s="12">
-        <f t="shared" si="1"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B24" s="12">
+        <v>1</v>
+      </c>
+      <c r="C24" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="C23" s="12">
-        <f t="shared" si="1"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B25" s="12">
+        <v>1</v>
+      </c>
+      <c r="C25" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="C24" s="12">
-        <f t="shared" si="1"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>58</v>
-      </c>
-      <c r="B25" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="C25" s="12">
-        <f t="shared" si="1"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="C26" s="12">
-        <f t="shared" si="1"/>
-        <v>0.6</v>
+      <c r="B26" s="12">
+        <v>1</v>
+      </c>
+      <c r="C26" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use chemicals industry temp demand as proxy for refining industry temp demand (#196)
</commit_message>
<xml_diff>
--- a/InputData/indst/IHDbT/Indst Heat Demand by Temp.xlsx
+++ b/InputData/indst/IHDbT/Indst Heat Demand by Temp.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\indst\IHDbT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\indst\IHDbT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C93C8E-FEF1-4AF0-944B-3A32143010E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701F05AA-FA92-484D-AA7E-49E8D10DE8D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9AA6BDF2-7B91-4567-88A2-0D83F9E3E450}"/>
+    <workbookView xWindow="16425" yWindow="1830" windowWidth="25815" windowHeight="19845" xr2:uid="{9AA6BDF2-7B91-4567-88A2-0D83F9E3E450}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
-    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="CH4_to_CO2e">'[1]Cross-Page Data'!$C$12</definedName>
@@ -29,9 +28,9 @@
     <definedName name="cpi_2013to2012">#REF!</definedName>
     <definedName name="cpi_2014to2012">#REF!</definedName>
     <definedName name="cpi_2016to2012">#REF!</definedName>
-    <definedName name="gigwatts_to_megawatts">[3]About!$A$31</definedName>
+    <definedName name="gigwatts_to_megawatts">[2]About!$A$31</definedName>
     <definedName name="N2O_to_CO2e">'[1]Cross-Page Data'!$C$13</definedName>
-    <definedName name="unit_conv">[4]About!$A$123</definedName>
+    <definedName name="unit_conv">[3]About!$A$123</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
@@ -338,7 +337,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -368,6 +367,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -3554,101 +3554,6 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Table of Contents"/>
-      <sheetName val="Indst Fuel Switching"/>
-      <sheetName val="Hydrogen Production"/>
-      <sheetName val="F-gases"/>
-      <sheetName val="Non-f-gas Process Emissions"/>
-      <sheetName val="Indst Efficiency"/>
-      <sheetName val="Industry CCS"/>
-      <sheetName val="Material Efficiency"/>
-      <sheetName val="CES"/>
-      <sheetName val="Battery Storage"/>
-      <sheetName val="Transmission"/>
-      <sheetName val="Demand Response"/>
-      <sheetName val="Coal regs"/>
-      <sheetName val="Gas regs"/>
-      <sheetName val="Nuclear subsidy"/>
-      <sheetName val="ITC and PTC"/>
-      <sheetName val="ZEV std"/>
-      <sheetName val="EV Tax Credits"/>
-      <sheetName val="Trans fuel econ"/>
-      <sheetName val="Mode shifting"/>
-      <sheetName val="EV charging"/>
-      <sheetName val="Bldg Electrification"/>
-      <sheetName val="Bldg Rebates"/>
-      <sheetName val="Bldg Retrofits"/>
-      <sheetName val="Bldg Efficiency"/>
-      <sheetName val="Forest Policies"/>
-      <sheetName val="Supporting Data --&gt;"/>
-      <sheetName val="NREL Indst"/>
-      <sheetName val="AEO 2021 Table 5"/>
-      <sheetName val="AEO 2021 Table 6"/>
-      <sheetName val="AEO 2021 Table 7"/>
-      <sheetName val="AEO 2021 Table 21"/>
-      <sheetName val="AEO 2021 Table 22"/>
-      <sheetName val="AEO 2021 Table 39"/>
-      <sheetName val="AEO 2018 Table 47"/>
-      <sheetName val="AEO 2017 Table 7"/>
-      <sheetName val="AEO 2017 Table 50"/>
-      <sheetName val="AEO2015 Table 7"/>
-      <sheetName val="AEO20212 Table 7"/>
-      <sheetName val="EIA Appl Data"/>
-      <sheetName val="USCA HFCs"/>
-      <sheetName val="Conversion Factors"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
       <sheetName val="About"/>
       <sheetName val="2035 Report Deployment"/>
       <sheetName val="2035 Report Data"/>
@@ -3682,7 +3587,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -4042,21 +3947,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE5FEEC-01CE-4291-999E-35B30A1256CF}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="85.08984375" customWidth="1"/>
+    <col min="2" max="2" width="85.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>62</v>
       </c>
@@ -4064,37 +3967,37 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="14">
         <v>2016</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -4114,45 +4017,45 @@
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" customWidth="1"/>
-    <col min="2" max="5" width="12.81640625" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="5" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>10</v>
       </c>
@@ -4169,7 +4072,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -4186,7 +4089,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -4203,7 +4106,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -4220,7 +4123,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>18</v>
       </c>
@@ -4237,7 +4140,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -4254,7 +4157,7 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>20</v>
       </c>
@@ -4271,7 +4174,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>21</v>
       </c>
@@ -4288,7 +4191,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>22</v>
       </c>
@@ -4305,12 +4208,12 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>24</v>
       </c>
@@ -4318,7 +4221,7 @@
         <v>115.5</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>25</v>
       </c>
@@ -4326,7 +4229,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>26</v>
       </c>
@@ -4335,7 +4238,7 @@
         <v>5.1948051948051948</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>27</v>
       </c>
@@ -4350,7 +4253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
         <v>29</v>
       </c>
@@ -4358,17 +4261,17 @@
         <v>0.27777800000000002</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>10</v>
       </c>
@@ -4385,7 +4288,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>31</v>
       </c>
@@ -4406,7 +4309,7 @@
         <v>826.59674132000964</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f t="shared" ref="A63:A70" si="0">A40</f>
         <v>Iron &amp; Steel</v>
@@ -4428,7 +4331,7 @@
         <v>56.103851220815123</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
         <f t="shared" si="0"/>
         <v>Nonmetallic Minerals</v>
@@ -4450,7 +4353,7 @@
         <v>28.051925610407562</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f t="shared" si="0"/>
         <v>Chemicals</v>
@@ -4472,7 +4375,7 @@
         <v>280.51925610407562</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f t="shared" si="0"/>
         <v>Nonferrous Metals</v>
@@ -4494,7 +4397,7 @@
         <v>28.051925610407562</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f t="shared" si="0"/>
         <v>Food &amp; Beverage</v>
@@ -4516,7 +4419,7 @@
         <v>211.32450626507031</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f t="shared" si="0"/>
         <v>Pulp &amp; Paper</v>
@@ -4538,7 +4441,7 @@
         <v>97.246675449412891</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f t="shared" si="0"/>
         <v>Machinery &amp; Vehicles</v>
@@ -4560,7 +4463,7 @@
         <v>41.14282422859776</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f t="shared" si="0"/>
         <v>Other Industries</v>
@@ -4593,19 +4496,17 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:B13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.26953125" customWidth="1"/>
+    <col min="1" max="1" width="46.28515625" customWidth="1"/>
     <col min="2" max="3" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -4616,7 +4517,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -4628,7 +4529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -4641,7 +4542,7 @@
         <v>0.24590163934426235</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -4654,7 +4555,7 @@
         <v>0.24590163934426235</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -4667,7 +4568,7 @@
         <v>0.24590163934426235</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -4680,7 +4581,7 @@
         <v>0.18772563176895307</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -4693,7 +4594,7 @@
         <v>0.24590163934426235</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -4706,7 +4607,7 @@
         <v>0.24590163934426235</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -4719,20 +4620,20 @@
         <v>6.4655172413793149E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="11">
-        <f>$B$23</f>
-        <v>0.75409836065573765</v>
+      <c r="B10" s="17">
+        <f>B11</f>
+        <v>0.31293463143254524</v>
       </c>
       <c r="C10" s="10">
         <f t="shared" si="0"/>
-        <v>0.24590163934426235</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0.68706536856745482</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -4745,7 +4646,7 @@
         <v>0.68706536856745482</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -4758,7 +4659,7 @@
         <v>0.24590163934426235</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -4771,7 +4672,7 @@
         <v>0.24590163934426235</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -4784,7 +4685,7 @@
         <v>0.87942122186495175</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -4797,7 +4698,7 @@
         <v>0.96990972918756269</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -4810,7 +4711,7 @@
         <v>0.76530612244897955</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -4823,7 +4724,7 @@
         <v>0.24590163934426235</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -4836,7 +4737,7 @@
         <v>0.24590163934426235</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -4849,7 +4750,7 @@
         <v>0.24590163934426235</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -4862,7 +4763,7 @@
         <v>0.16666666666666663</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>52</v>
       </c>
@@ -4875,7 +4776,7 @@
         <v>0.16666666666666663</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -4888,7 +4789,7 @@
         <v>0.16666666666666663</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -4901,7 +4802,7 @@
         <v>0.24590163934426235</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -4913,7 +4814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -4925,7 +4826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>57</v>
       </c>
@@ -4936,6 +4837,9 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Analysis for emissions by temperature range
</commit_message>
<xml_diff>
--- a/InputData/indst/IHDbT/Indst Heat Demand by Temp.xlsx
+++ b/InputData/indst/IHDbT/Indst Heat Demand by Temp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\indst\IHDbT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\indst\IHDbT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701F05AA-FA92-484D-AA7E-49E8D10DE8D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A960BA88-5A6C-49BD-A914-DB47D50D7AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16425" yWindow="1830" windowWidth="25815" windowHeight="19845" xr2:uid="{9AA6BDF2-7B91-4567-88A2-0D83F9E3E450}"/>
+    <workbookView xWindow="-27165" yWindow="1725" windowWidth="25095" windowHeight="14130" activeTab="1" xr2:uid="{9AA6BDF2-7B91-4567-88A2-0D83F9E3E450}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <definedName name="N2O_to_CO2e">'[1]Cross-Page Data'!$C$13</definedName>
     <definedName name="unit_conv">[3]About!$A$123</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="66">
   <si>
     <t>IHDbT Industrial Heat Demand by Temperature</t>
   </si>
@@ -231,9 +231,6 @@
     <t>Perc Low Temp</t>
   </si>
   <si>
-    <t>Perc Medium and High Temp</t>
-  </si>
-  <si>
     <t>We assume the fraction of low temp heat is 100% for the agriculture, natural gas processing, water and waste,</t>
   </si>
   <si>
@@ -247,6 +244,12 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Per Medium Temp</t>
+  </si>
+  <si>
+    <t>Perc High Temp</t>
   </si>
 </sst>
 </file>
@@ -337,7 +340,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -353,7 +356,6 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3449,7 +3451,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="About"/>
@@ -3551,7 +3553,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="About"/>
@@ -3588,7 +3590,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="About"/>
@@ -3947,7 +3949,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE5FEEC-01CE-4291-999E-35B30A1256CF}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3961,45 +3965,45 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="14">
+      <c r="B4" s="13">
         <v>2016</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -4015,7 +4019,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADCAD35F-524E-466F-828E-86F7D1F08980}">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4496,183 +4502,235 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46.28515625" customWidth="1"/>
-    <col min="2" max="3" width="28" customWidth="1"/>
+    <col min="2" max="4" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="11">
         <v>1</v>
       </c>
-      <c r="C2" s="10">
-        <f t="shared" ref="C2:C14" si="0">1-B2</f>
+      <c r="C2" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="10">
+        <f t="shared" ref="D2:D22" si="0">1-B2-C2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="11">
-        <f>$B$23</f>
+      <c r="B3" s="10">
+        <f>B23</f>
         <v>0.75409836065573765</v>
       </c>
       <c r="C3" s="10">
+        <f>C23</f>
+        <v>0.24590163934426229</v>
+      </c>
+      <c r="D3" s="10">
         <f t="shared" si="0"/>
-        <v>0.24590163934426235</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="11">
-        <f t="shared" ref="B4:B5" si="1">$B$23</f>
+      <c r="B4" s="10">
+        <f>B23</f>
         <v>0.75409836065573765</v>
       </c>
       <c r="C4" s="10">
+        <f>C23</f>
+        <v>0.24590163934426229</v>
+      </c>
+      <c r="D4" s="10">
         <f t="shared" si="0"/>
-        <v>0.24590163934426235</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="11">
-        <f t="shared" si="1"/>
+      <c r="B5" s="10">
+        <f>B23</f>
         <v>0.75409836065573765</v>
       </c>
       <c r="C5" s="10">
+        <f>C23</f>
+        <v>0.24590163934426229</v>
+      </c>
+      <c r="D5" s="10">
         <f t="shared" si="0"/>
-        <v>0.24590163934426235</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="10">
         <f>SUM(Data!D67:E67)/SUM(Data!B67:E67)</f>
         <v>0.81227436823104693</v>
       </c>
       <c r="C6" s="10">
+        <f>SUM(Data!C67)/SUM(Data!B67:E67)</f>
+        <v>0.10830324909747291</v>
+      </c>
+      <c r="D6" s="10">
         <f t="shared" si="0"/>
-        <v>0.18772563176895307</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7.9422382671480163E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="11">
-        <f>$B$23</f>
+      <c r="B7" s="10">
+        <f>B23</f>
         <v>0.75409836065573765</v>
       </c>
       <c r="C7" s="10">
+        <f>C23</f>
+        <v>0.24590163934426229</v>
+      </c>
+      <c r="D7" s="10">
         <f t="shared" si="0"/>
-        <v>0.24590163934426235</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="11">
-        <f>$B$23</f>
+      <c r="B8" s="10">
+        <f>B23</f>
         <v>0.75409836065573765</v>
       </c>
       <c r="C8" s="10">
+        <f>C23</f>
+        <v>0.24590163934426229</v>
+      </c>
+      <c r="D8" s="10">
         <f t="shared" si="0"/>
-        <v>0.24590163934426235</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="10">
         <f>SUM(Data!D68:E68)/SUM(Data!B68:E68)</f>
         <v>0.93534482758620685</v>
       </c>
       <c r="C9" s="10">
+        <f>SUM(Data!C68)/SUM(Data!B68:E68)</f>
+        <v>4.9568965517241374E-2</v>
+      </c>
+      <c r="D9" s="10">
         <f t="shared" si="0"/>
-        <v>6.4655172413793149E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.5086206896551775E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="16">
         <f>B11</f>
         <v>0.31293463143254524</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="16">
+        <f>C11</f>
+        <v>2.0862308762169681E-2</v>
+      </c>
+      <c r="D10" s="10">
         <f t="shared" si="0"/>
-        <v>0.68706536856745482</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.66620305980528516</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="10">
         <f>SUM(Data!D65:E65)/SUM(Data!B65:E65)</f>
         <v>0.31293463143254524</v>
       </c>
       <c r="C11" s="10">
+        <f>SUM(Data!C65)/SUM(Data!B65:E65)</f>
+        <v>2.0862308762169681E-2</v>
+      </c>
+      <c r="D11" s="10">
         <f t="shared" si="0"/>
-        <v>0.68706536856745482</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.66620305980528516</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="11">
-        <f>$B$23</f>
+      <c r="B12" s="10">
+        <f>B23</f>
         <v>0.75409836065573765</v>
       </c>
       <c r="C12" s="10">
+        <f>C23</f>
+        <v>0.24590163934426229</v>
+      </c>
+      <c r="D12" s="10">
         <f t="shared" si="0"/>
-        <v>0.24590163934426235</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="11">
-        <f>$B$23</f>
+      <c r="B13" s="10">
+        <f>B23</f>
         <v>0.75409836065573765</v>
       </c>
       <c r="C13" s="10">
+        <f>C23</f>
+        <v>0.24590163934426229</v>
+      </c>
+      <c r="D13" s="10">
         <f t="shared" si="0"/>
-        <v>0.24590163934426235</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -4681,11 +4739,15 @@
         <v>0.12057877813504822</v>
       </c>
       <c r="C14" s="10">
+        <f>SUM(Data!C64)/SUM(Data!B64:E64)</f>
+        <v>0.14469453376205788</v>
+      </c>
+      <c r="D14" s="10">
         <f t="shared" si="0"/>
-        <v>0.87942122186495175</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.73472668810289388</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -4694,152 +4756,198 @@
         <v>3.0090270812437311E-2</v>
       </c>
       <c r="C15" s="10">
-        <f>1-B15</f>
-        <v>0.96990972918756269</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <f>SUM(Data!C63)/SUM(Data!B63:E63)</f>
+        <v>3.0090270812437311E-2</v>
+      </c>
+      <c r="D15" s="10">
+        <f t="shared" si="0"/>
+        <v>0.93981945837512537</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="10">
         <f>SUM(Data!D66:E66)/SUM(Data!B66:E66)</f>
         <v>0.23469387755102042</v>
       </c>
       <c r="C16" s="10">
-        <f t="shared" ref="C16:C26" si="2">1-B16</f>
-        <v>0.76530612244897955</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <f>SUM(Data!C66)/SUM(Data!B66:E66)</f>
+        <v>0.30612244897959184</v>
+      </c>
+      <c r="D16" s="10">
+        <f t="shared" si="0"/>
+        <v>0.45918367346938771</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="11">
-        <f>$B$23</f>
+      <c r="B17" s="10">
+        <f>B23</f>
         <v>0.75409836065573765</v>
       </c>
       <c r="C17" s="10">
-        <f t="shared" si="2"/>
-        <v>0.24590163934426235</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <f>C23</f>
+        <v>0.24590163934426229</v>
+      </c>
+      <c r="D17" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="11">
-        <f t="shared" ref="B18:B19" si="3">$B$23</f>
+      <c r="B18" s="10">
+        <f>B23</f>
         <v>0.75409836065573765</v>
       </c>
       <c r="C18" s="10">
-        <f t="shared" si="2"/>
-        <v>0.24590163934426235</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <f>C23</f>
+        <v>0.24590163934426229</v>
+      </c>
+      <c r="D18" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="11">
-        <f t="shared" si="3"/>
+      <c r="B19" s="10">
+        <f>B23</f>
         <v>0.75409836065573765</v>
       </c>
       <c r="C19" s="10">
-        <f t="shared" si="2"/>
-        <v>0.24590163934426235</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <f>C23</f>
+        <v>0.24590163934426229</v>
+      </c>
+      <c r="D19" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="10">
         <f>SUM(Data!D69:E69)/SUM(Data!B69:E69)</f>
         <v>0.83333333333333337</v>
       </c>
       <c r="C20" s="10">
-        <f t="shared" si="2"/>
-        <v>0.16666666666666663</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <f>SUM(Data!C69)/SUM(Data!B69:E69)</f>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="D20" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="11">
-        <f>$B$20</f>
+      <c r="B21" s="10">
+        <f>B20</f>
         <v>0.83333333333333337</v>
       </c>
       <c r="C21" s="10">
-        <f t="shared" si="2"/>
-        <v>0.16666666666666663</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <f>C20</f>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="D21" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="11">
-        <f>$B$20</f>
+      <c r="B22" s="10">
+        <f>B20</f>
         <v>0.83333333333333337</v>
       </c>
       <c r="C22" s="10">
-        <f t="shared" si="2"/>
-        <v>0.16666666666666663</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <f>C20</f>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="D22" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B23" s="10">
         <f>SUM(Data!D70:E70)/SUM(Data!B70:E70)</f>
         <v>0.75409836065573765</v>
       </c>
       <c r="C23" s="10">
-        <f t="shared" si="2"/>
-        <v>0.24590163934426235</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <f>SUM(Data!C70)/SUM(Data!B70:E70)</f>
+        <v>0.24590163934426229</v>
+      </c>
+      <c r="D23" s="10">
+        <f>1-B23-C23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B24" s="11">
         <v>1</v>
       </c>
-      <c r="C24" s="10">
-        <f t="shared" si="2"/>
+      <c r="C24" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="10">
+        <f t="shared" ref="D24:D26" si="1">1-B24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="12">
+      <c r="B25" s="11">
         <v>1</v>
       </c>
-      <c r="C25" s="10">
-        <f t="shared" si="2"/>
+      <c r="C25" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B26" s="11">
         <v>1</v>
       </c>
-      <c r="C26" s="10">
-        <f t="shared" si="2"/>
+      <c r="C26" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>